<commit_message>
Payment Method Change 20160105
Paypal First;
Remove loginId in tbl_customer_login_info;
</commit_message>
<xml_diff>
--- a/02_Management/功能.xlsx
+++ b/02_Management/功能.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="195" windowWidth="19395" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16480"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schedule!$A$4:$J$30</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -275,223 +280,223 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>优先顺：3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优先顺：4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_GB_CA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_GB_OL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_GB_OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_TP_LG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_CS_PE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_CS_OL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_CS_OD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecommerce_orders.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单一览</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单详细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecommerce_orders_view.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团购一览</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团购详细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品一览</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品详细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecommerce_products.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecommerce_products_edit.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_MN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_LG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_AA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_OL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_OD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_PL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_PD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_GL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OZ_TT_AD_GD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreditCardPayment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlipayPayment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WeChatPayment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PayPalPayment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI Reference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login-page.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg-page.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该页面的风格类似登陆页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内容如下：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重复密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子邮件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forgotton-password.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过手机号码验证重置/通过电子邮件验证重置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优先顺：2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>优先顺：1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>优先顺：2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>优先顺：3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>优先顺：4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_GB_CA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_GB_OL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_GB_OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_TP_LG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_CS_PE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_CS_OL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_CS_OD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ecommerce_orders.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单一览</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单详细</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ecommerce_orders_view.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团购一览</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团购详细</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品一览</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品详细</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ecommerce_products.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ecommerce_products_edit.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主界面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_MN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_LG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_AA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_OL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_OD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_PL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_PD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_GL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OZ_TT_AD_GD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreditCardPayment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AlipayPayment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WeChatPayment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PayPalPayment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI Reference</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login-page.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg-page.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>该页面的风格类似登陆页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>内容如下：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重复密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>电子邮件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>forgotton-password.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分Tab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过手机号码验证重置/通过电子邮件验证重置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -578,16 +583,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,20 +601,20 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,33 +622,33 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -652,7 +657,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -660,33 +665,33 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,15 +738,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,9 +762,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3305,65 +3310,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="18.625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="1" customWidth="1"/>
+    <col min="8" max="10" width="18.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="16" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:10" ht="16" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="12" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+    <row r="3" spans="1:10" ht="16" customHeight="1">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+    <row r="4" spans="1:10" ht="16" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="9" t="s">
         <v>45</v>
       </c>
@@ -3371,30 +3376,30 @@
         <v>44</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="16" customHeight="1">
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>49</v>
@@ -3405,14 +3410,14 @@
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="16" customHeight="1">
       <c r="A6" s="3">
         <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="4" t="s">
         <v>31</v>
       </c>
@@ -3426,14 +3431,14 @@
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="16" customHeight="1">
       <c r="A7" s="3">
         <f t="shared" ref="A7:A30" si="0">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
@@ -3447,14 +3452,14 @@
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="16" customHeight="1">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="4" t="s">
         <v>33</v>
       </c>
@@ -3468,23 +3473,23 @@
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="16" customHeight="1">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
@@ -3495,19 +3500,19 @@
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="16" customHeight="1">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>53</v>
@@ -3516,19 +3521,19 @@
       <c r="I10" s="6"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="16" customHeight="1">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>52</v>
@@ -3537,39 +3542,39 @@
       <c r="I11" s="6"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="16" customHeight="1">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="20" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="16" customHeight="1">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
@@ -3577,7 +3582,7 @@
         <v>57</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>23</v>
@@ -3585,14 +3590,14 @@
       <c r="I13" s="6"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="16" customHeight="1">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="4" t="s">
         <v>39</v>
       </c>
@@ -3600,7 +3605,7 @@
         <v>58</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>27</v>
@@ -3608,107 +3613,107 @@
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="16" customHeight="1">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="16" customHeight="1">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="5" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="16" customHeight="1">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="13"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="16" customHeight="1">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="16" customHeight="1">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -3718,7 +3723,7 @@
         <v>40</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>53</v>
@@ -3729,21 +3734,21 @@
       <c r="I19" s="6"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="16" customHeight="1">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>53</v>
@@ -3754,19 +3759,19 @@
       <c r="I20" s="6"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="16" customHeight="1">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>53</v>
@@ -3775,25 +3780,25 @@
       <c r="I21" s="6"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="16" customHeight="1">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>47</v>
@@ -3804,68 +3809,68 @@
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="16" customHeight="1">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="s">
-        <v>70</v>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="6"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="16" customHeight="1">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="16" customHeight="1">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="20" t="s">
         <v>20</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>25</v>
@@ -3873,88 +3878,88 @@
       <c r="I25" s="6"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="16" customHeight="1">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="6"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="16" customHeight="1">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="6"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="16" customHeight="1">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="6"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="16" customHeight="1">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5" t="s">
@@ -3963,19 +3968,19 @@
       <c r="I29" s="6"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="16" customHeight="1">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -3984,6 +3989,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="H2:J4"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="B5:B21"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:D4"/>
     <mergeCell ref="E2:G3"/>
@@ -3999,17 +4011,15 @@
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="H2:J4"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="B5:B21"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4017,17 +4027,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="2.875" style="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="2.83203125" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4035,9 +4050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
@@ -4045,6 +4060,11 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4056,49 +4076,54 @@
       <selection activeCell="B2" sqref="B2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="E6" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B4" s="1" t="s">
+    <row r="8" spans="2:5">
+      <c r="E8" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="E6" s="1" t="s">
+    <row r="10" spans="2:5">
+      <c r="E10" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="E8" s="1" t="s">
+    <row r="12" spans="2:5">
+      <c r="E12" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="E10" s="1" t="s">
+    <row r="14" spans="2:5">
+      <c r="E14" s="1" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="E12" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="E14" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4108,34 +4133,39 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="D6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:5">
       <c r="E8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4143,11 +4173,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
@@ -4155,6 +4185,11 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4162,9 +4197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
@@ -4172,5 +4207,10 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>